<commit_message>
Wells and Edelman also works. Finally understand animation with functools.partial and init_func!
</commit_message>
<xml_diff>
--- a/Projects/Wells/cases/TheisHantush/TheisHantush.xlsx
+++ b/Projects/Wells/cases/TheisHantush/TheisHantush.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/GRWMODELS/python/mf6lab/Projects/Wells/cases/TheisHantush/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3E7BA6-3F14-2346-836B-2DF887365B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE13F3B0-E000-6D47-B8F5-876D8D4B792E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="6720" windowWidth="30600" windowHeight="19860" tabRatio="751" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="2540" windowWidth="30600" windowHeight="19860" tabRatio="751" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NAM" sheetId="1" r:id="rId1"/>
@@ -11878,10 +11878,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="C3" s="10">
-        <v>365</v>
+        <v>30</v>
       </c>
       <c r="D3" s="10">
         <v>1</v>

</xml_diff>